<commit_message>
Duty cycle and windings are updated
</commit_message>
<xml_diff>
--- a/Magnetic Design.xlsx
+++ b/Magnetic Design.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Desktop\EE464\METU-EE464-TermProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yorga\Desktop\ee464 project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28A4E4A2-1355-4E99-A8D4-A8B568180441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E7B5B3E-2F1A-4177-9B28-A40E833C682B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13440" yWindow="3375" windowWidth="18000" windowHeight="9300" xr2:uid="{4A373523-0C95-434F-A770-35848E385085}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4A373523-0C95-434F-A770-35848E385085}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -496,25 +496,25 @@
   <dimension ref="C3:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="37.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>17</v>
       </c>
@@ -522,7 +522,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>19</v>
       </c>
@@ -530,7 +530,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>11</v>
       </c>
@@ -542,7 +542,7 @@
       </c>
       <c r="H6">
         <f>(D15*D19)/((D14*1000)*(D6*0.000001)*(2*D7))</f>
-        <v>1.423728813559322</v>
+        <v>1.0610169491525425</v>
       </c>
       <c r="J6" t="s">
         <v>21</v>
@@ -555,7 +555,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>1</v>
       </c>
@@ -567,21 +567,21 @@
       </c>
       <c r="H7">
         <f>H6*D24</f>
-        <v>1.0677966101694916</v>
+        <v>1.0610169491525425</v>
       </c>
       <c r="J7" s="2">
         <f>8/H6</f>
-        <v>5.6190476190476195</v>
+        <v>7.5399361022364211</v>
       </c>
       <c r="L7" t="s">
         <v>23</v>
       </c>
       <c r="M7">
         <f>H7*J7</f>
-        <v>6.0000000000000009</v>
-      </c>
-    </row>
-    <row r="8" spans="3:13" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
         <v>24</v>
       </c>
@@ -590,7 +590,7 @@
         <v>375.55</v>
       </c>
     </row>
-    <row r="9" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>25</v>
       </c>
@@ -602,10 +602,10 @@
       </c>
       <c r="H9">
         <f>((M6+M7)*D27*D28)/D8</f>
-        <v>0.11183597390493942</v>
-      </c>
-    </row>
-    <row r="10" spans="3:13" x14ac:dyDescent="0.25">
+        <v>0.12781254160564506</v>
+      </c>
+    </row>
+    <row r="10" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
         <v>27</v>
       </c>
@@ -613,7 +613,7 @@
         <v>17.2</v>
       </c>
     </row>
-    <row r="11" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
         <v>28</v>
       </c>
@@ -621,12 +621,12 @@
         <v>18.5</v>
       </c>
     </row>
-    <row r="13" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C13" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
         <v>12</v>
       </c>
@@ -638,38 +638,38 @@
       </c>
       <c r="H14">
         <f>2*D24*D16*D19</f>
-        <v>15.120000000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="3:13" x14ac:dyDescent="0.25">
+        <v>15.071999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
         <v>16</v>
       </c>
       <c r="D15">
-        <v>0.42</v>
+        <v>0.313</v>
       </c>
       <c r="G15" t="s">
         <v>13</v>
       </c>
       <c r="H15">
         <f>2*D24*D15*D20</f>
-        <v>15.120000000000001</v>
-      </c>
-    </row>
-    <row r="16" spans="3:13" x14ac:dyDescent="0.25">
+        <v>15.024000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
         <v>15</v>
       </c>
       <c r="D16">
-        <v>0.21</v>
-      </c>
-    </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+        <v>0.157</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C18" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
         <v>4</v>
       </c>
@@ -677,7 +677,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
         <v>5</v>
       </c>
@@ -685,7 +685,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C21" t="s">
         <v>6</v>
       </c>
@@ -693,25 +693,25 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C23" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C24" t="s">
         <v>9</v>
       </c>
       <c r="D24">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C26" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C27" t="s">
         <v>30</v>
       </c>
@@ -719,7 +719,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C28" t="s">
         <v>31</v>
       </c>

</xml_diff>